<commit_message>
read me and github icone
</commit_message>
<xml_diff>
--- a/data/Data_growth_EPX_DMX.xlsx
+++ b/data/Data_growth_EPX_DMX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisagollot/Library/CloudStorage/OneDrive-Personnel/Documents/0_These/0_RepoGit/Ew-Growth-IdVar/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124D9852-07B3-CA46-85B3-3881C408610B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C104E3-ADCD-144A-B330-07DEBFC96F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30600" yWindow="-3000" windowWidth="25860" windowHeight="15900" activeTab="1" xr2:uid="{B6F91018-2402-2E49-89F8-0A687BF48367}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{B6F91018-2402-2E49-89F8-0A687BF48367}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="8" r:id="rId1"/>
@@ -875,10 +875,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98193405-CF40-6248-94AF-85C31E4AA383}">
-  <dimension ref="A1:K301"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L315" sqref="L315"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -894,7 +895,7 @@
     <col min="9" max="9" width="40.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -923,7 +924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>45063</v>
       </c>
@@ -950,7 +951,7 @@
       </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>45063</v>
       </c>
@@ -977,7 +978,7 @@
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>45063</v>
       </c>
@@ -1004,7 +1005,7 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>45063</v>
       </c>
@@ -1031,7 +1032,7 @@
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>45063</v>
       </c>
@@ -1058,7 +1059,7 @@
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>45063</v>
       </c>
@@ -1085,7 +1086,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>45063</v>
       </c>
@@ -1111,8 +1112,12 @@
         <v>0</v>
       </c>
       <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f>AVERAGE(G2:G61)</f>
+        <v>12.424999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>45063</v>
       </c>
@@ -1139,7 +1144,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>45063</v>
       </c>
@@ -1170,7 +1175,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>45063</v>
       </c>
@@ -1197,7 +1202,7 @@
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>45063</v>
       </c>
@@ -1224,7 +1229,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>45063</v>
       </c>
@@ -1251,7 +1256,7 @@
       </c>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>45063</v>
       </c>
@@ -1278,7 +1283,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>45063</v>
       </c>
@@ -1305,7 +1310,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>45063</v>
       </c>
@@ -2522,7 +2527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>45043</v>
       </c>
@@ -2549,7 +2554,7 @@
       </c>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>45077</v>
       </c>
@@ -2574,7 +2579,7 @@
       </c>
       <c r="I62" s="5"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>45077</v>
       </c>
@@ -2602,7 +2607,7 @@
       </c>
       <c r="I63" s="7"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>45077</v>
       </c>
@@ -2630,7 +2635,7 @@
       </c>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>45077</v>
       </c>
@@ -2658,7 +2663,7 @@
       </c>
       <c r="I65" s="7"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>45077</v>
       </c>
@@ -2686,7 +2691,7 @@
       </c>
       <c r="I66" s="7"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>45077</v>
       </c>
@@ -2714,7 +2719,7 @@
       </c>
       <c r="I67" s="7"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>45077</v>
       </c>
@@ -2742,7 +2747,7 @@
       </c>
       <c r="I68" s="7"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>45077</v>
       </c>
@@ -2770,7 +2775,7 @@
       </c>
       <c r="I69" s="7"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>45077</v>
       </c>
@@ -2796,7 +2801,7 @@
       </c>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>45077</v>
       </c>
@@ -2824,7 +2829,7 @@
       </c>
       <c r="I71" s="7"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>45077</v>
       </c>
@@ -2852,7 +2857,7 @@
       </c>
       <c r="I72" s="7"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>45077</v>
       </c>
@@ -2880,7 +2885,7 @@
       </c>
       <c r="I73" s="7"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>45077</v>
       </c>
@@ -2908,7 +2913,7 @@
       </c>
       <c r="I74" s="7"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>45077</v>
       </c>
@@ -2936,7 +2941,7 @@
       </c>
       <c r="I75" s="7"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>45077</v>
       </c>
@@ -2964,7 +2969,7 @@
       </c>
       <c r="I76" s="7"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>45077</v>
       </c>
@@ -2992,7 +2997,7 @@
       </c>
       <c r="I77" s="7"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>45077</v>
       </c>
@@ -3020,7 +3025,7 @@
       </c>
       <c r="I78" s="7"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>45077</v>
       </c>
@@ -3048,7 +3053,7 @@
       </c>
       <c r="I79" s="7"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>45077</v>
       </c>
@@ -3076,7 +3081,7 @@
       </c>
       <c r="I80" s="7"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>45077</v>
       </c>
@@ -3104,7 +3109,7 @@
       </c>
       <c r="I81" s="7"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>45077</v>
       </c>
@@ -3132,7 +3137,7 @@
       </c>
       <c r="I82" s="7"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>45077</v>
       </c>
@@ -3160,7 +3165,7 @@
       </c>
       <c r="I83" s="7"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>45077</v>
       </c>
@@ -3188,7 +3193,7 @@
       </c>
       <c r="I84" s="7"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <v>45077</v>
       </c>
@@ -3216,7 +3221,7 @@
       </c>
       <c r="I85" s="7"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <v>45077</v>
       </c>
@@ -3244,7 +3249,7 @@
       </c>
       <c r="I86" s="7"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <v>45077</v>
       </c>
@@ -3272,7 +3277,7 @@
       </c>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
         <v>45077</v>
       </c>
@@ -3300,7 +3305,7 @@
       </c>
       <c r="I88" s="7"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
         <v>45077</v>
       </c>
@@ -3326,7 +3331,7 @@
       </c>
       <c r="I89" s="7"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>45077</v>
       </c>
@@ -3354,7 +3359,7 @@
       </c>
       <c r="I90" s="7"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
         <v>45077</v>
       </c>
@@ -3382,7 +3387,7 @@
       </c>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>45057</v>
       </c>
@@ -3410,7 +3415,7 @@
       </c>
       <c r="I92" s="7"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>45057</v>
       </c>
@@ -3438,7 +3443,7 @@
       </c>
       <c r="I93" s="7"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>45057</v>
       </c>
@@ -3464,7 +3469,7 @@
       </c>
       <c r="I94" s="7"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>45057</v>
       </c>
@@ -3492,7 +3497,7 @@
       </c>
       <c r="I95" s="7"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
         <v>45057</v>
       </c>
@@ -3520,7 +3525,7 @@
       </c>
       <c r="I96" s="7"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
         <v>45057</v>
       </c>
@@ -3548,7 +3553,7 @@
       </c>
       <c r="I97" s="7"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
         <v>45057</v>
       </c>
@@ -3576,7 +3581,7 @@
       </c>
       <c r="I98" s="7"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
         <v>45057</v>
       </c>
@@ -3604,7 +3609,7 @@
       </c>
       <c r="I99" s="7"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
         <v>45057</v>
       </c>
@@ -3632,7 +3637,7 @@
       </c>
       <c r="I100" s="7"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>45057</v>
       </c>
@@ -3660,7 +3665,7 @@
       </c>
       <c r="I101" s="7"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>45057</v>
       </c>
@@ -3686,7 +3691,7 @@
       </c>
       <c r="I102" s="7"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>45057</v>
       </c>
@@ -3714,7 +3719,7 @@
       </c>
       <c r="I103" s="7"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>45057</v>
       </c>
@@ -3742,7 +3747,7 @@
       </c>
       <c r="I104" s="7"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>45057</v>
       </c>
@@ -3770,7 +3775,7 @@
       </c>
       <c r="I105" s="7"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>45057</v>
       </c>
@@ -3798,7 +3803,7 @@
       </c>
       <c r="I106" s="7"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6">
         <v>45057</v>
       </c>
@@ -3826,7 +3831,7 @@
       </c>
       <c r="I107" s="7"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6">
         <v>45057</v>
       </c>
@@ -3854,7 +3859,7 @@
       </c>
       <c r="I108" s="7"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <v>45057</v>
       </c>
@@ -3882,7 +3887,7 @@
       </c>
       <c r="I109" s="7"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6">
         <v>45057</v>
       </c>
@@ -3910,7 +3915,7 @@
       </c>
       <c r="I110" s="7"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6">
         <v>45057</v>
       </c>
@@ -3938,7 +3943,7 @@
       </c>
       <c r="I111" s="7"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
         <v>45057</v>
       </c>
@@ -3966,7 +3971,7 @@
       </c>
       <c r="I112" s="7"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6">
         <v>45057</v>
       </c>
@@ -3994,7 +3999,7 @@
       </c>
       <c r="I113" s="7"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
         <v>45057</v>
       </c>
@@ -4022,7 +4027,7 @@
       </c>
       <c r="I114" s="7"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>45057</v>
       </c>
@@ -4050,7 +4055,7 @@
       </c>
       <c r="I115" s="7"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <v>45057</v>
       </c>
@@ -4078,7 +4083,7 @@
       </c>
       <c r="I116" s="7"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6">
         <v>45057</v>
       </c>
@@ -4106,7 +4111,7 @@
       </c>
       <c r="I117" s="7"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6">
         <v>45057</v>
       </c>
@@ -4132,7 +4137,7 @@
       </c>
       <c r="I118" s="7"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6">
         <v>45057</v>
       </c>
@@ -4160,7 +4165,7 @@
       </c>
       <c r="I119" s="7"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
         <v>45057</v>
       </c>
@@ -4186,7 +4191,7 @@
       </c>
       <c r="I120" s="7"/>
     </row>
-    <row r="121" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="22" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="8">
         <v>45057</v>
       </c>
@@ -4214,7 +4219,7 @@
       </c>
       <c r="I121" s="10"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="14">
         <v>45091</v>
       </c>
@@ -4239,7 +4244,7 @@
       </c>
       <c r="I122" s="5"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="16">
         <v>45091</v>
       </c>
@@ -4267,7 +4272,7 @@
       </c>
       <c r="I123" s="7"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="16">
         <v>45091</v>
       </c>
@@ -4295,7 +4300,7 @@
       </c>
       <c r="I124" s="7"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="16">
         <v>45091</v>
       </c>
@@ -4323,7 +4328,7 @@
       </c>
       <c r="I125" s="7"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="16">
         <v>45091</v>
       </c>
@@ -4351,7 +4356,7 @@
       </c>
       <c r="I126" s="7"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="16">
         <v>45091</v>
       </c>
@@ -4379,7 +4384,7 @@
       </c>
       <c r="I127" s="7"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="16">
         <v>45091</v>
       </c>
@@ -4407,7 +4412,7 @@
       </c>
       <c r="I128" s="7"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="16">
         <v>45091</v>
       </c>
@@ -4435,7 +4440,7 @@
       </c>
       <c r="I129" s="7"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="16">
         <v>45091</v>
       </c>
@@ -4461,7 +4466,7 @@
       </c>
       <c r="I130" s="7"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="16">
         <v>45091</v>
       </c>
@@ -4489,7 +4494,7 @@
       </c>
       <c r="I131" s="7"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="16">
         <v>45091</v>
       </c>
@@ -4517,7 +4522,7 @@
       </c>
       <c r="I132" s="7"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="16">
         <v>45091</v>
       </c>
@@ -4545,7 +4550,7 @@
       </c>
       <c r="I133" s="7"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="16">
         <v>45091</v>
       </c>
@@ -4573,7 +4578,7 @@
       </c>
       <c r="I134" s="7"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="16">
         <v>45091</v>
       </c>
@@ -4601,7 +4606,7 @@
       </c>
       <c r="I135" s="7"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="16">
         <v>45091</v>
       </c>
@@ -4629,7 +4634,7 @@
       </c>
       <c r="I136" s="7"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="16">
         <v>45091</v>
       </c>
@@ -4657,7 +4662,7 @@
       </c>
       <c r="I137" s="7"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="16">
         <v>45091</v>
       </c>
@@ -4685,7 +4690,7 @@
       </c>
       <c r="I138" s="7"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="16">
         <v>45091</v>
       </c>
@@ -4713,7 +4718,7 @@
       </c>
       <c r="I139" s="7"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="16">
         <v>45091</v>
       </c>
@@ -4741,7 +4746,7 @@
       </c>
       <c r="I140" s="7"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="16">
         <v>45091</v>
       </c>
@@ -4769,7 +4774,7 @@
       </c>
       <c r="I141" s="7"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="16">
         <v>45091</v>
       </c>
@@ -4797,7 +4802,7 @@
       </c>
       <c r="I142" s="7"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="16">
         <v>45091</v>
       </c>
@@ -4825,7 +4830,7 @@
       </c>
       <c r="I143" s="7"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="16">
         <v>45091</v>
       </c>
@@ -4853,7 +4858,7 @@
       </c>
       <c r="I144" s="7"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="16">
         <v>45091</v>
       </c>
@@ -4881,7 +4886,7 @@
       </c>
       <c r="I145" s="7"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="16">
         <v>45091</v>
       </c>
@@ -4909,7 +4914,7 @@
       </c>
       <c r="I146" s="7"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="16">
         <v>45091</v>
       </c>
@@ -4937,7 +4942,7 @@
       </c>
       <c r="I147" s="7"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="16">
         <v>45091</v>
       </c>
@@ -4965,7 +4970,7 @@
       </c>
       <c r="I148" s="7"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="16">
         <v>45091</v>
       </c>
@@ -4991,7 +4996,7 @@
       </c>
       <c r="I149" s="7"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="16">
         <v>45091</v>
       </c>
@@ -5019,7 +5024,7 @@
       </c>
       <c r="I150" s="7"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <v>45091</v>
       </c>
@@ -5047,7 +5052,7 @@
       </c>
       <c r="I151" s="7"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="6">
         <v>45071</v>
       </c>
@@ -5075,7 +5080,7 @@
       </c>
       <c r="I152" s="7"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="6">
         <v>45071</v>
       </c>
@@ -5103,7 +5108,7 @@
       </c>
       <c r="I153" s="7"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6">
         <v>45071</v>
       </c>
@@ -5131,7 +5136,7 @@
       </c>
       <c r="I154" s="7"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6">
         <v>45071</v>
       </c>
@@ -5159,7 +5164,7 @@
       </c>
       <c r="I155" s="7"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="6">
         <v>45071</v>
       </c>
@@ -5187,7 +5192,7 @@
       </c>
       <c r="I156" s="7"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="6">
         <v>45071</v>
       </c>
@@ -5215,7 +5220,7 @@
       </c>
       <c r="I157" s="7"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="6">
         <v>45071</v>
       </c>
@@ -5243,7 +5248,7 @@
       </c>
       <c r="I158" s="7"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="6">
         <v>45071</v>
       </c>
@@ -5271,7 +5276,7 @@
       </c>
       <c r="I159" s="7"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6">
         <v>45071</v>
       </c>
@@ -5299,7 +5304,7 @@
       </c>
       <c r="I160" s="7"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="6">
         <v>45071</v>
       </c>
@@ -5327,7 +5332,7 @@
       </c>
       <c r="I161" s="7"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="6">
         <v>45071</v>
       </c>
@@ -5353,7 +5358,7 @@
       </c>
       <c r="I162" s="7"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="6">
         <v>45071</v>
       </c>
@@ -5381,7 +5386,7 @@
       </c>
       <c r="I163" s="7"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="6">
         <v>45071</v>
       </c>
@@ -5407,7 +5412,7 @@
       </c>
       <c r="I164" s="7"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="6">
         <v>45071</v>
       </c>
@@ -5435,7 +5440,7 @@
       </c>
       <c r="I165" s="7"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="6">
         <v>45071</v>
       </c>
@@ -5463,7 +5468,7 @@
       </c>
       <c r="I166" s="7"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="6">
         <v>45071</v>
       </c>
@@ -5491,7 +5496,7 @@
       </c>
       <c r="I167" s="7"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="6">
         <v>45071</v>
       </c>
@@ -5519,7 +5524,7 @@
       </c>
       <c r="I168" s="7"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="6">
         <v>45071</v>
       </c>
@@ -5547,7 +5552,7 @@
       </c>
       <c r="I169" s="7"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="6">
         <v>45071</v>
       </c>
@@ -5575,7 +5580,7 @@
       </c>
       <c r="I170" s="7"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="6">
         <v>45071</v>
       </c>
@@ -5603,7 +5608,7 @@
       </c>
       <c r="I171" s="7"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="6">
         <v>45071</v>
       </c>
@@ -5631,7 +5636,7 @@
       </c>
       <c r="I172" s="7"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="6">
         <v>45071</v>
       </c>
@@ -5659,7 +5664,7 @@
       </c>
       <c r="I173" s="7"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="6">
         <v>45071</v>
       </c>
@@ -5687,7 +5692,7 @@
       </c>
       <c r="I174" s="7"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="6">
         <v>45071</v>
       </c>
@@ -5715,7 +5720,7 @@
       </c>
       <c r="I175" s="7"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="6">
         <v>45071</v>
       </c>
@@ -5743,7 +5748,7 @@
       </c>
       <c r="I176" s="7"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="6">
         <v>45071</v>
       </c>
@@ -5771,7 +5776,7 @@
       </c>
       <c r="I177" s="7"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="6">
         <v>45071</v>
       </c>
@@ -5797,7 +5802,7 @@
       </c>
       <c r="I178" s="7"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="6">
         <v>45071</v>
       </c>
@@ -5825,7 +5830,7 @@
       </c>
       <c r="I179" s="7"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="6">
         <v>45071</v>
       </c>
@@ -5851,7 +5856,7 @@
       </c>
       <c r="I180" s="7"/>
     </row>
-    <row r="181" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" ht="22" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="6">
         <v>45071</v>
       </c>
@@ -5879,7 +5884,7 @@
       </c>
       <c r="I181" s="10"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="14">
         <v>45105</v>
       </c>
@@ -5904,7 +5909,7 @@
       </c>
       <c r="I182" s="5"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="16">
         <v>45105</v>
       </c>
@@ -5932,7 +5937,7 @@
       </c>
       <c r="I183" s="7"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="16">
         <v>45105</v>
       </c>
@@ -5960,7 +5965,7 @@
       </c>
       <c r="I184" s="7"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="16">
         <v>45105</v>
       </c>
@@ -5988,7 +5993,7 @@
       </c>
       <c r="I185" s="7"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="16">
         <v>45105</v>
       </c>
@@ -6016,7 +6021,7 @@
       </c>
       <c r="I186" s="7"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="16">
         <v>45105</v>
       </c>
@@ -6044,7 +6049,7 @@
       </c>
       <c r="I187" s="7"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="16">
         <v>45105</v>
       </c>
@@ -6072,7 +6077,7 @@
       </c>
       <c r="I188" s="7"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="16">
         <v>45105</v>
       </c>
@@ -6100,7 +6105,7 @@
       </c>
       <c r="I189" s="7"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="16">
         <v>45105</v>
       </c>
@@ -6126,7 +6131,7 @@
       </c>
       <c r="I190" s="7"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="16">
         <v>45105</v>
       </c>
@@ -6154,7 +6159,7 @@
       </c>
       <c r="I191" s="7"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="16">
         <v>45105</v>
       </c>
@@ -6182,7 +6187,7 @@
       </c>
       <c r="I192" s="7"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="16">
         <v>45105</v>
       </c>
@@ -6210,7 +6215,7 @@
       </c>
       <c r="I193" s="7"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="16">
         <v>45105</v>
       </c>
@@ -6238,7 +6243,7 @@
       </c>
       <c r="I194" s="7"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="16">
         <v>45105</v>
       </c>
@@ -6266,7 +6271,7 @@
       </c>
       <c r="I195" s="7"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="16">
         <v>45105</v>
       </c>
@@ -6294,7 +6299,7 @@
       </c>
       <c r="I196" s="7"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="16">
         <v>45105</v>
       </c>
@@ -6322,7 +6327,7 @@
       </c>
       <c r="I197" s="7"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="16">
         <v>45105</v>
       </c>
@@ -6350,7 +6355,7 @@
       </c>
       <c r="I198" s="7"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="16">
         <v>45105</v>
       </c>
@@ -6378,7 +6383,7 @@
       </c>
       <c r="I199" s="7"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="16">
         <v>45105</v>
       </c>
@@ -6406,7 +6411,7 @@
       </c>
       <c r="I200" s="7"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="16">
         <v>45105</v>
       </c>
@@ -6434,7 +6439,7 @@
       </c>
       <c r="I201" s="7"/>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="16">
         <v>45105</v>
       </c>
@@ -6462,7 +6467,7 @@
       </c>
       <c r="I202" s="7"/>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="16">
         <v>45105</v>
       </c>
@@ -6490,7 +6495,7 @@
       </c>
       <c r="I203" s="7"/>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="16">
         <v>45105</v>
       </c>
@@ -6518,7 +6523,7 @@
       </c>
       <c r="I204" s="7"/>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="16">
         <v>45105</v>
       </c>
@@ -6546,7 +6551,7 @@
       </c>
       <c r="I205" s="7"/>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="16">
         <v>45105</v>
       </c>
@@ -6574,7 +6579,7 @@
       </c>
       <c r="I206" s="7"/>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="16">
         <v>45105</v>
       </c>
@@ -6602,7 +6607,7 @@
       </c>
       <c r="I207" s="7"/>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="16">
         <v>45105</v>
       </c>
@@ -6630,7 +6635,7 @@
       </c>
       <c r="I208" s="7"/>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="16">
         <v>45105</v>
       </c>
@@ -6656,7 +6661,7 @@
       </c>
       <c r="I209" s="7"/>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="16">
         <v>45105</v>
       </c>
@@ -6684,7 +6689,7 @@
       </c>
       <c r="I210" s="7"/>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="16">
         <v>45105</v>
       </c>
@@ -6712,7 +6717,7 @@
       </c>
       <c r="I211" s="7"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="6">
         <v>45085</v>
       </c>
@@ -6740,7 +6745,7 @@
       </c>
       <c r="I212" s="7"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="6">
         <v>45085</v>
       </c>
@@ -6770,7 +6775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="6">
         <v>45085</v>
       </c>
@@ -6798,7 +6803,7 @@
       </c>
       <c r="I214" s="7"/>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="6">
         <v>45085</v>
       </c>
@@ -6826,7 +6831,7 @@
       </c>
       <c r="I215" s="7"/>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="6">
         <v>45085</v>
       </c>
@@ -6854,7 +6859,7 @@
       </c>
       <c r="I216" s="7"/>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="6">
         <v>45085</v>
       </c>
@@ -6882,7 +6887,7 @@
       </c>
       <c r="I217" s="7"/>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="6">
         <v>45085</v>
       </c>
@@ -6908,7 +6913,7 @@
       </c>
       <c r="I218" s="7"/>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="6">
         <v>45085</v>
       </c>
@@ -6936,7 +6941,7 @@
       </c>
       <c r="I219" s="7"/>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="6">
         <v>45085</v>
       </c>
@@ -6964,7 +6969,7 @@
       </c>
       <c r="I220" s="7"/>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="6">
         <v>45085</v>
       </c>
@@ -6992,7 +6997,7 @@
       </c>
       <c r="I221" s="7"/>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="6">
         <v>45085</v>
       </c>
@@ -7018,7 +7023,7 @@
       </c>
       <c r="I222" s="7"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="6">
         <v>45085</v>
       </c>
@@ -7046,7 +7051,7 @@
       </c>
       <c r="I223" s="7"/>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="6">
         <v>45085</v>
       </c>
@@ -7072,7 +7077,7 @@
       </c>
       <c r="I224" s="7"/>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="6">
         <v>45085</v>
       </c>
@@ -7100,7 +7105,7 @@
       </c>
       <c r="I225" s="7"/>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="6">
         <v>45085</v>
       </c>
@@ -7128,7 +7133,7 @@
       </c>
       <c r="I226" s="7"/>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="6">
         <v>45085</v>
       </c>
@@ -7156,7 +7161,7 @@
       </c>
       <c r="I227" s="7"/>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="6">
         <v>45085</v>
       </c>
@@ -7184,7 +7189,7 @@
       </c>
       <c r="I228" s="7"/>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="6">
         <v>45085</v>
       </c>
@@ -7212,7 +7217,7 @@
       </c>
       <c r="I229" s="7"/>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="6">
         <v>45085</v>
       </c>
@@ -7240,7 +7245,7 @@
       </c>
       <c r="I230" s="7"/>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="6">
         <v>45085</v>
       </c>
@@ -7268,7 +7273,7 @@
       </c>
       <c r="I231" s="7"/>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="6">
         <v>45085</v>
       </c>
@@ -7296,7 +7301,7 @@
       </c>
       <c r="I232" s="7"/>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="6">
         <v>45085</v>
       </c>
@@ -7324,7 +7329,7 @@
       </c>
       <c r="I233" s="7"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="6">
         <v>45085</v>
       </c>
@@ -7352,7 +7357,7 @@
       </c>
       <c r="I234" s="7"/>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="6">
         <v>45085</v>
       </c>
@@ -7380,7 +7385,7 @@
       </c>
       <c r="I235" s="7"/>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="6">
         <v>45085</v>
       </c>
@@ -7408,7 +7413,7 @@
       </c>
       <c r="I236" s="7"/>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="6">
         <v>45085</v>
       </c>
@@ -7436,7 +7441,7 @@
       </c>
       <c r="I237" s="7"/>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="6">
         <v>45085</v>
       </c>
@@ -7462,7 +7467,7 @@
       </c>
       <c r="I238" s="7"/>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="6">
         <v>45085</v>
       </c>
@@ -7490,7 +7495,7 @@
       </c>
       <c r="I239" s="7"/>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="6">
         <v>45085</v>
       </c>
@@ -7516,7 +7521,7 @@
       </c>
       <c r="I240" s="7"/>
     </row>
-    <row r="241" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" ht="22" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="6">
         <v>45085</v>
       </c>
@@ -7544,7 +7549,7 @@
       </c>
       <c r="I241" s="10"/>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="14">
         <v>45119</v>
       </c>
@@ -7569,7 +7574,7 @@
       </c>
       <c r="I242" s="5"/>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="6">
         <v>45119</v>
       </c>
@@ -7597,7 +7602,7 @@
       </c>
       <c r="I243" s="7"/>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="6">
         <v>45119</v>
       </c>
@@ -7625,7 +7630,7 @@
       </c>
       <c r="I244" s="7"/>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="6">
         <v>45119</v>
       </c>
@@ -7653,7 +7658,7 @@
       </c>
       <c r="I245" s="7"/>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="6">
         <v>45119</v>
       </c>
@@ -7681,7 +7686,7 @@
       </c>
       <c r="I246" s="7"/>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="6">
         <v>45119</v>
       </c>
@@ -7709,7 +7714,7 @@
       </c>
       <c r="I247" s="7"/>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="6">
         <v>45119</v>
       </c>
@@ -7737,7 +7742,7 @@
       </c>
       <c r="I248" s="7"/>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="6">
         <v>45119</v>
       </c>
@@ -7765,7 +7770,7 @@
       </c>
       <c r="I249" s="7"/>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="6">
         <v>45119</v>
       </c>
@@ -7791,7 +7796,7 @@
       </c>
       <c r="I250" s="7"/>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="6">
         <v>45119</v>
       </c>
@@ -7819,7 +7824,7 @@
       </c>
       <c r="I251" s="7"/>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="6">
         <v>45119</v>
       </c>
@@ -7847,7 +7852,7 @@
       </c>
       <c r="I252" s="7"/>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="6">
         <v>45119</v>
       </c>
@@ -7875,7 +7880,7 @@
       </c>
       <c r="I253" s="7"/>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="6">
         <v>45119</v>
       </c>
@@ -7903,7 +7908,7 @@
       </c>
       <c r="I254" s="7"/>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="6">
         <v>45119</v>
       </c>
@@ -7931,7 +7936,7 @@
       </c>
       <c r="I255" s="7"/>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="6">
         <v>45119</v>
       </c>
@@ -7959,7 +7964,7 @@
       </c>
       <c r="I256" s="7"/>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="6">
         <v>45119</v>
       </c>
@@ -7987,7 +7992,7 @@
       </c>
       <c r="I257" s="7"/>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="6">
         <v>45119</v>
       </c>
@@ -8015,7 +8020,7 @@
       </c>
       <c r="I258" s="7"/>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="6">
         <v>45119</v>
       </c>
@@ -8043,7 +8048,7 @@
       </c>
       <c r="I259" s="7"/>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="6">
         <v>45119</v>
       </c>
@@ -8071,7 +8076,7 @@
       </c>
       <c r="I260" s="7"/>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="6">
         <v>45119</v>
       </c>
@@ -8099,7 +8104,7 @@
       </c>
       <c r="I261" s="7"/>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="6">
         <v>45119</v>
       </c>
@@ -8127,7 +8132,7 @@
       </c>
       <c r="I262" s="7"/>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="6">
         <v>45119</v>
       </c>
@@ -8155,7 +8160,7 @@
       </c>
       <c r="I263" s="7"/>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="6">
         <v>45119</v>
       </c>
@@ -8183,7 +8188,7 @@
       </c>
       <c r="I264" s="7"/>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="6">
         <v>45119</v>
       </c>
@@ -8211,7 +8216,7 @@
       </c>
       <c r="I265" s="7"/>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="6">
         <v>45119</v>
       </c>
@@ -8239,7 +8244,7 @@
       </c>
       <c r="I266" s="7"/>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="6">
         <v>45119</v>
       </c>
@@ -8267,7 +8272,7 @@
       </c>
       <c r="I267" s="7"/>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="6">
         <v>45119</v>
       </c>
@@ -8295,7 +8300,7 @@
       </c>
       <c r="I268" s="7"/>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="6">
         <v>45119</v>
       </c>
@@ -8321,7 +8326,7 @@
       </c>
       <c r="I269" s="7"/>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="6">
         <v>45119</v>
       </c>
@@ -8349,7 +8354,7 @@
       </c>
       <c r="I270" s="7"/>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="6">
         <v>45119</v>
       </c>
@@ -8377,7 +8382,7 @@
       </c>
       <c r="I271" s="7"/>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="6">
         <v>45099</v>
       </c>
@@ -8405,7 +8410,7 @@
       </c>
       <c r="I272" s="7"/>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="6">
         <v>45099</v>
       </c>
@@ -8433,7 +8438,7 @@
       </c>
       <c r="I273" s="7"/>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="6">
         <v>45099</v>
       </c>
@@ -8461,7 +8466,7 @@
       </c>
       <c r="I274" s="7"/>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="6">
         <v>45099</v>
       </c>
@@ -8489,7 +8494,7 @@
       </c>
       <c r="I275" s="7"/>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="6">
         <v>45099</v>
       </c>
@@ -8517,7 +8522,7 @@
       </c>
       <c r="I276" s="7"/>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="6">
         <v>45099</v>
       </c>
@@ -8545,7 +8550,7 @@
       </c>
       <c r="I277" s="7"/>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="6">
         <v>45099</v>
       </c>
@@ -8571,7 +8576,7 @@
       </c>
       <c r="I278" s="7"/>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="6">
         <v>45099</v>
       </c>
@@ -8599,7 +8604,7 @@
       </c>
       <c r="I279" s="7"/>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="6">
         <v>45099</v>
       </c>
@@ -8627,7 +8632,7 @@
       </c>
       <c r="I280" s="7"/>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="6">
         <v>45099</v>
       </c>
@@ -8655,7 +8660,7 @@
       </c>
       <c r="I281" s="7"/>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="6">
         <v>45099</v>
       </c>
@@ -8681,7 +8686,7 @@
       </c>
       <c r="I282" s="7"/>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="6">
         <v>45099</v>
       </c>
@@ -8709,7 +8714,7 @@
       </c>
       <c r="I283" s="7"/>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="6">
         <v>45099</v>
       </c>
@@ -8735,7 +8740,7 @@
       </c>
       <c r="I284" s="7"/>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="6">
         <v>45099</v>
       </c>
@@ -8763,7 +8768,7 @@
       </c>
       <c r="I285" s="7"/>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="6">
         <v>45099</v>
       </c>
@@ -8791,7 +8796,7 @@
       </c>
       <c r="I286" s="7"/>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="6">
         <v>45099</v>
       </c>
@@ -8819,7 +8824,7 @@
       </c>
       <c r="I287" s="7"/>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="6">
         <v>45099</v>
       </c>
@@ -8847,7 +8852,7 @@
       </c>
       <c r="I288" s="7"/>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="6">
         <v>45099</v>
       </c>
@@ -8875,7 +8880,7 @@
       </c>
       <c r="I289" s="7"/>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="6">
         <v>45099</v>
       </c>
@@ -8903,7 +8908,7 @@
       </c>
       <c r="I290" s="7"/>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="6">
         <v>45099</v>
       </c>
@@ -8931,7 +8936,7 @@
       </c>
       <c r="I291" s="7"/>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="6">
         <v>45099</v>
       </c>
@@ -8959,7 +8964,7 @@
       </c>
       <c r="I292" s="7"/>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="6">
         <v>45099</v>
       </c>
@@ -8987,7 +8992,7 @@
       </c>
       <c r="I293" s="7"/>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="6">
         <v>45099</v>
       </c>
@@ -9015,7 +9020,7 @@
       </c>
       <c r="I294" s="7"/>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="6">
         <v>45099</v>
       </c>
@@ -9043,7 +9048,7 @@
       </c>
       <c r="I295" s="7"/>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="6">
         <v>45099</v>
       </c>
@@ -9071,7 +9076,7 @@
       </c>
       <c r="I296" s="7"/>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="6">
         <v>45099</v>
       </c>
@@ -9099,7 +9104,7 @@
       </c>
       <c r="I297" s="7"/>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="6">
         <v>45099</v>
       </c>
@@ -9125,7 +9130,7 @@
       </c>
       <c r="I298" s="7"/>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="6">
         <v>45099</v>
       </c>
@@ -9153,7 +9158,7 @@
       </c>
       <c r="I299" s="7"/>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="6">
         <v>45099</v>
       </c>
@@ -9179,7 +9184,7 @@
       </c>
       <c r="I300" s="7"/>
     </row>
-    <row r="301" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" ht="22" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="8">
         <v>45099</v>
       </c>
@@ -9208,7 +9213,13 @@
       <c r="I301" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I301" xr:uid="{98193405-CF40-6248-94AF-85C31E4AA383}"/>
+  <autoFilter ref="A1:I301" xr:uid="{98193405-CF40-6248-94AF-85C31E4AA383}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1000</formula>

</xml_diff>